<commit_message>
Updated bulk upload sample & default files
</commit_message>
<xml_diff>
--- a/MDO/client-assets/assets/common/user-approvals-upload-sample/user-approvals-upload-sample.xlsx
+++ b/MDO/client-assets/assets/common/user-approvals-upload-sample/user-approvals-upload-sample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IGOT_NIC\Assets\forked\sunbird-cb-portal-assets\MDO\client-assets\assets\common\user-approvals-upload-sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD9C6D44-5E6C-4420-91C8-2479E10D8177}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C594D7C-678E-4168-9864-6F4DD0D401EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="732" yWindow="1920" windowWidth="22308" windowHeight="10140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,79 +30,79 @@
     <t>Email</t>
   </si>
   <si>
+    <t>Designation</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>Employee ID</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Tags</t>
+  </si>
+  <si>
+    <t>Sahil Chaudhary</t>
+  </si>
+  <si>
+    <t>123C</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>OBC</t>
+  </si>
+  <si>
+    <t>USER12345</t>
+  </si>
+  <si>
+    <t>Group A</t>
+  </si>
+  <si>
+    <t>27-07-1998</t>
+  </si>
+  <si>
+    <t>ACCOUNTANT</t>
+  </si>
+  <si>
     <t xml:space="preserve"> Mobile Number</t>
   </si>
   <si>
     <t>Full Name</t>
   </si>
   <si>
-    <t>Designation</t>
-  </si>
-  <si>
-    <t>Group</t>
-  </si>
-  <si>
-    <t>Employee ID</t>
-  </si>
-  <si>
-    <t>Gender</t>
-  </si>
-  <si>
-    <t>Date of birth</t>
-  </si>
-  <si>
-    <t>Mother tongue</t>
-  </si>
-  <si>
-    <t>Category</t>
-  </si>
-  <si>
-    <t>Office Pin code</t>
-  </si>
-  <si>
-    <t>eHRMS ID</t>
+    <t>Date Of Birth (dd-mm-yyyy)</t>
+  </si>
+  <si>
+    <t>Mother Tongue</t>
+  </si>
+  <si>
+    <t>Office Pin Code</t>
   </si>
   <si>
     <t>External System Name</t>
   </si>
   <si>
-    <t>Tags</t>
-  </si>
-  <si>
-    <t>sahilTest11@yopmail.com</t>
-  </si>
-  <si>
-    <t>Sahil Chaudhary</t>
-  </si>
-  <si>
-    <t>Accountant Director</t>
-  </si>
-  <si>
-    <t>123C</t>
-  </si>
-  <si>
-    <t>Male</t>
-  </si>
-  <si>
-    <t>27-7-1998</t>
-  </si>
-  <si>
-    <t>English</t>
-  </si>
-  <si>
-    <t>OBC</t>
-  </si>
-  <si>
-    <t>USER12345</t>
-  </si>
-  <si>
-    <t>Test File</t>
-  </si>
-  <si>
-    <t>Sahil,Shyave</t>
-  </si>
-  <si>
-    <t>Group A</t>
+    <t>External System ID</t>
+  </si>
+  <si>
+    <t>sahil11@yopmail.com</t>
+  </si>
+  <si>
+    <t>Rozgar Mela, Finance</t>
+  </si>
+  <si>
+    <t>eHRMSN</t>
   </si>
 </sst>
 </file>
@@ -147,10 +147,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -536,111 +541,112 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.44140625" customWidth="1"/>
-    <col min="2" max="2" width="14.109375" customWidth="1"/>
-    <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="12.5546875" customWidth="1"/>
-    <col min="6" max="6" width="26.5546875" customWidth="1"/>
-    <col min="7" max="7" width="24" customWidth="1"/>
-    <col min="8" max="8" width="19.5546875" customWidth="1"/>
+    <col min="1" max="1" width="24.33203125" customWidth="1"/>
+    <col min="2" max="2" width="28.44140625" customWidth="1"/>
+    <col min="3" max="3" width="14.5546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5546875" customWidth="1"/>
+    <col min="5" max="5" width="13.21875" customWidth="1"/>
+    <col min="6" max="6" width="9.88671875" customWidth="1"/>
+    <col min="7" max="7" width="10.5546875" customWidth="1"/>
+    <col min="8" max="8" width="22.109375" customWidth="1"/>
     <col min="9" max="9" width="12.5546875" customWidth="1"/>
-    <col min="10" max="10" width="10.5546875" customWidth="1"/>
-    <col min="11" max="11" width="23.33203125" customWidth="1"/>
-    <col min="12" max="12" width="18.33203125" customWidth="1"/>
+    <col min="10" max="10" width="11.109375" customWidth="1"/>
+    <col min="11" max="11" width="12.88671875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="17.44140625" customWidth="1"/>
     <col min="13" max="13" width="20.5546875" customWidth="1"/>
-    <col min="14" max="14" width="9.109375" customWidth="1"/>
+    <col min="14" max="14" width="25.109375" customWidth="1"/>
     <col min="15" max="15" width="9.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="K1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N1" t="s">
         <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="1">
+        <v>7894561230</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" t="s">
         <v>14</v>
       </c>
-      <c r="B2">
-        <v>1922221142</v>
-      </c>
-      <c r="C2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H2" t="s">
-        <v>19</v>
-      </c>
       <c r="I2" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="J2" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="K2" s="2">
         <v>201010</v>
       </c>
       <c r="L2" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="M2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="N2" t="s">
         <v>24</v>
@@ -648,7 +654,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>